<commit_message>
Added some images to break block of texts
</commit_message>
<xml_diff>
--- a/src/figures/meres.xlsx
+++ b/src/figures/meres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korpos\study\thesis-template-latex\src\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C98554-63BB-4534-AC6D-B33ED2B898DB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DBF551-AE7E-48BA-9335-8A41748BFD49}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{B4A51D0A-8BE4-4294-8CC8-5EF1F6B18E83}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="11">
   <si>
     <t>Egyszerű állapotgép</t>
   </si>
@@ -232,7 +232,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Munka1!$B$5:$G$5</c:f>
+              <c:f>Munka1!$B$1:$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -607,14 +607,16 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>Futási</a:t>
+              <a:rPr lang="hu-HU" sz="1600" b="1" baseline="0">
+                <a:latin typeface="+mn-lt"/>
+                <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              </a:rPr>
+              <a:t>Futási idő az állapotok száma szerint</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="hu-HU" baseline="0"/>
-              <a:t> idők őrfeltételekkel</a:t>
-            </a:r>
-            <a:endParaRPr lang="hu-HU"/>
+            <a:endParaRPr lang="hu-HU" sz="1600" b="1">
+              <a:latin typeface="+mn-lt"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -654,26 +656,21 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10012756704167165"/>
-          <c:y val="0.12386642270238411"/>
-          <c:w val="0.86854423770865918"/>
-          <c:h val="0.63132473976001047"/>
+          <c:x val="0.11858992278301353"/>
+          <c:y val="0.12748146837033769"/>
+          <c:w val="0.84163227459107526"/>
+          <c:h val="0.70580152579128574"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Őrfeltételek nélkül</c:v>
-          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -693,158 +690,82 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Munka2!$B$5:$G$5</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>m1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>m2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>m3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>m4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>m5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>m6</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
-              <c:f>Munka2!$B$6:$G$6</c:f>
+              <c:f>Munka1!$B$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>541</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>541</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>575</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>726</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>885</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1281</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-5E7E-4AFC-A0C3-03079F722513}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Őrfeltételekkel</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Munka2!$B$5:$G$5</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>m1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>m2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>m3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>m4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>m5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>m6</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Munka2!$B$7:$G$7</c:f>
+              <c:f>Munka1!$B$6:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>623</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>612</c:v>
+                  <c:v>537</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>660</c:v>
+                  <c:v>571</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>953</c:v>
+                  <c:v>704</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1148</c:v>
+                  <c:v>877</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1784</c:v>
+                  <c:v>1316</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-5E7E-4AFC-A0C3-03079F722513}"/>
+              <c16:uniqueId val="{00000000-F0B8-4CB3-B829-B35009A6A320}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -852,18 +773,32 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1121455248"/>
-        <c:axId val="1161259728"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1121455248"/>
+        <c:axId val="1663949504"/>
+        <c:axId val="1679934320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1663949504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2100"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -884,12 +819,25 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="hu-HU"/>
-                  <a:t>modell</a:t>
+                  <a:rPr lang="hu-HU" sz="1600"/>
+                  <a:t>Állapotok</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="hu-HU" sz="1600" baseline="0"/>
+                  <a:t> száma</a:t>
+                </a:r>
+                <a:endParaRPr lang="hu-HU" sz="1600"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.37957828623270812"/>
+              <c:y val="0.91122860728086452"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -919,7 +867,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -928,8 +876,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -941,7 +889,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -956,18 +904,16 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1161259728"/>
+        <c:crossAx val="1679934320"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="200"/>
+        <c:minorUnit val="20"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1161259728"/>
+        <c:axId val="1679934320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1900"/>
           <c:min val="400"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1006,17 +952,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="hu-HU"/>
-                  <a:t>futási</a:t>
+                  <a:rPr lang="hu-HU" sz="1600"/>
+                  <a:t>Futási idő (ms)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="hu-HU" baseline="0"/>
-                  <a:t> idő (ms)</a:t>
-                </a:r>
-                <a:endParaRPr lang="hu-HU"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="8.2432976748500323E-4"/>
+              <c:y val="0.31678515496507342"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1052,6 +1001,611 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1663949504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="hu-HU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hu-HU" sz="1600" b="1"/>
+              <a:t>Futási</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="hu-HU" sz="1600" b="1" baseline="0"/>
+              <a:t> idők őrfeltételekkel</a:t>
+            </a:r>
+            <a:endParaRPr lang="hu-HU" sz="1600" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11573224718576505"/>
+          <c:y val="0.12386640050275406"/>
+          <c:w val="0.84947191198687844"/>
+          <c:h val="0.61536548895243504"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Őrfeltételek nélkül</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka2!$B$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka2!$B$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>541</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>541</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>885</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1281</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5E7E-4AFC-A0C3-03079F722513}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Őrfeltételekkel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka2!$B$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka2!$B$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>623</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>612</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>953</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1148</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1784</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5E7E-4AFC-A0C3-03079F722513}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1121455248"/>
+        <c:axId val="1161259728"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1121455248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU" sz="1600"/>
+                  <a:t>állapotok száma</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.3987025589762675"/>
+              <c:y val="0.80185452722024209"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1161259728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="200"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1161259728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1900"/>
+          <c:min val="400"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU" sz="1600"/>
+                  <a:t>futási</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="hu-HU" sz="1600" baseline="0"/>
+                  <a:t> idő (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="hu-HU" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="5.6613721796555938E-3"/>
+              <c:y val="0.32622472367010463"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
           <a:ln>
             <a:noFill/>
           </a:ln>
@@ -1062,7 +1616,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1079,7 +1633,7 @@
         </c:txPr>
         <c:crossAx val="1121455248"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1097,8 +1651,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.2319841312275513E-2"/>
           <c:y val="0.8571364349691275"/>
-          <c:w val="0.22082135485805884"/>
-          <c:h val="0.11749429493637056"/>
+          <c:w val="0.24499428374522128"/>
+          <c:h val="0.14286364806808788"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1254,6 +1808,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1758,7 +2352,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1785,8 +2379,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1887,7 +2481,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1919,6 +2513,522 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
     <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
@@ -2264,16 +3374,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2356,6 +3466,42 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171448</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Diagram 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64639D9C-DF24-4A28-AA89-0037F3C06116}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2363,16 +3509,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>257176</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2699,8 +3845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629F826B-58EB-40A8-AC04-CA8EC7F2C0D5}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2712,6 +3858,24 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2783,23 +3947,29 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="B5">
+        <f>B2</f>
         <v>10</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:G5" si="0">C2</f>
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>2000</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2835,8 +4005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDFA3FB0-A0CD-48E8-97D4-69D67EC54F70}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>